<commit_message>
Excel BOM shows whole of schematic sheet 1 has been checked
</commit_message>
<xml_diff>
--- a/Hardware/Cornverter BOM 2019 02 09.xlsx
+++ b/Hardware/Cornverter BOM 2019 02 09.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!!Product Design\Cornverter\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{61A95727-1C29-42CC-B0AF-B94694F7EA28}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0868864D-DBD1-4620-AF97-D3B5D6094845}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cornverter BOM 2019 02 09" sheetId="1" r:id="rId1"/>
@@ -726,7 +726,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1574,12 +1574,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E27" sqref="E27"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2675,37 +2675,37 @@
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>1</v>
-      </c>
-      <c r="B33" s="2" t="s">
+    <row r="33" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="3">
+        <v>1</v>
+      </c>
+      <c r="B33" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G33" s="2"/>
-      <c r="H33" s="2"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="2"/>
-      <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="2"/>
-      <c r="O33" s="2"/>
-      <c r="P33" s="2"/>
-      <c r="Q33" s="2"/>
-      <c r="R33" s="2"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="3"/>
+      <c r="J33" s="3"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
+      <c r="N33" s="3"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
@@ -3830,7 +3830,7 @@
       <c r="R67" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R67">
+  <autoFilter ref="A1:R67" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R67">
       <sortCondition ref="D1:D67"/>
     </sortState>

</xml_diff>

<commit_message>
Checked Over all of schematic sheet 2: Power
</commit_message>
<xml_diff>
--- a/Hardware/Cornverter BOM 2019 02 09.xlsx
+++ b/Hardware/Cornverter BOM 2019 02 09.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!!Product Design\Cornverter\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0868864D-DBD1-4620-AF97-D3B5D6094845}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942B50E4-62D0-4046-BC2A-6021A0C17B0B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -719,7 +719,37 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> C6, C7, C9, C10, C11, C20, C21, C24, C25, C27, C28</t>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C6, C7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, C9, C10, C11, C20, C21, C24, C25, C27, C28, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C26</t>
     </r>
   </si>
 </sst>
@@ -1578,8 +1608,8 @@
   <dimension ref="A1:R67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E33" sqref="E33"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1645,37 +1675,37 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+    <row r="2" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -1709,37 +1739,37 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>1</v>
-      </c>
-      <c r="B4" s="2" t="s">
+    <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -2329,7 +2359,7 @@
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>79</v>
@@ -2573,39 +2603,39 @@
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+    <row r="30" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
         <v>3</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2"/>
-      <c r="I30" s="2"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="2"/>
-      <c r="O30" s="2"/>
-      <c r="P30" s="2"/>
-      <c r="Q30" s="2" t="s">
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="3"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="R30" s="2"/>
+      <c r="R30" s="3"/>
     </row>
     <row r="31" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
@@ -3105,37 +3135,37 @@
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+    <row r="46" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
         <v>2</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C46" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D46" s="2" t="s">
+      <c r="D46" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="E46" s="2" t="s">
+      <c r="E46" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F46" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
-      <c r="O46" s="2"/>
-      <c r="P46" s="2"/>
-      <c r="Q46" s="2"/>
-      <c r="R46" s="2"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3"/>
+      <c r="O46" s="3"/>
+      <c r="P46" s="3"/>
+      <c r="Q46" s="3"/>
+      <c r="R46" s="3"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
@@ -3179,47 +3209,47 @@
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
-        <v>1</v>
-      </c>
-      <c r="B48" s="2" t="s">
+    <row r="48" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>1</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C48" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D48" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="E48" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F48" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G48" s="2" t="s">
+      <c r="G48" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="H48" s="2" t="s">
+      <c r="H48" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="I48" s="2" t="s">
+      <c r="I48" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="J48" s="2" t="s">
+      <c r="J48" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2" t="s">
+      <c r="K48" s="3"/>
+      <c r="L48" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
-      <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
-      <c r="Q48" s="2"/>
-      <c r="R48" s="2"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3"/>
+      <c r="O48" s="3"/>
+      <c r="P48" s="3"/>
+      <c r="Q48" s="3"/>
+      <c r="R48" s="3"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="2">

</xml_diff>

<commit_message>
Changed value of R3 (on the MCU side of the 6n138) from 220 to 280 ohms as per midi spec
</commit_message>
<xml_diff>
--- a/Hardware/Cornverter BOM 2019 02 09.xlsx
+++ b/Hardware/Cornverter BOM 2019 02 09.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!!Product Design\Cornverter\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{942B50E4-62D0-4046-BC2A-6021A0C17B0B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA86655-6ACA-4AD2-8F3D-E3091BA3F978}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Cornverter BOM 2019 02 09" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cornverter BOM 2019 02 09'!$A$1:$R$67</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Cornverter BOM 2019 02 09'!$A$1:$R$68</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="221">
   <si>
     <t>Qty</t>
   </si>
@@ -458,9 +458,6 @@
   </si>
   <si>
     <t>1M</t>
-  </si>
-  <si>
-    <t>R3, R4</t>
   </si>
   <si>
     <t>22K</t>
@@ -751,6 +748,12 @@
       </rPr>
       <t>C26</t>
     </r>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R3</t>
   </si>
 </sst>
 </file>
@@ -1605,11 +1608,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R67"/>
+  <dimension ref="A1:R68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="154" zoomScaleNormal="154" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2371,7 +2374,7 @@
         <v>81</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>82</v>
@@ -2802,45 +2805,45 @@
       <c r="R35" s="2"/>
     </row>
     <row r="36" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="3">
-        <v>2</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="C36" s="3" t="s">
+      <c r="A36" s="2">
+        <v>1</v>
+      </c>
+      <c r="B36" s="2">
+        <v>220</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="F36" s="3" t="s">
+      <c r="E36" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
-      <c r="M36" s="3"/>
-      <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
-      <c r="P36" s="3"/>
-      <c r="Q36" s="3" t="s">
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="2"/>
+      <c r="L36" s="2"/>
+      <c r="M36" s="2"/>
+      <c r="N36" s="2"/>
+      <c r="O36" s="2"/>
+      <c r="P36" s="2"/>
+      <c r="Q36" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="R36" s="3"/>
+      <c r="R36" s="2"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>2</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>138</v>
+        <v>1</v>
+      </c>
+      <c r="B37" s="2">
+        <v>280</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>133</v>
@@ -2849,7 +2852,7 @@
         <v>134</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>139</v>
+        <v>220</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>136</v>
@@ -2870,77 +2873,79 @@
       <c r="R37" s="2"/>
     </row>
     <row r="38" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="3">
-        <v>1</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="C38" s="3" t="s">
+      <c r="A38" s="2">
+        <v>16</v>
+      </c>
+      <c r="B38" s="2">
+        <v>330</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="F38" s="3" t="s">
+      <c r="E38" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3"/>
-      <c r="L38" s="3"/>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
-      <c r="R38" s="3"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="2"/>
+      <c r="L38" s="2"/>
+      <c r="M38" s="2"/>
+      <c r="N38" s="2"/>
+      <c r="O38" s="2"/>
+      <c r="P38" s="2"/>
+      <c r="Q38" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="R38" s="2"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <v>22</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="C39" s="2" t="s">
+      <c r="A39" s="3">
+        <v>2</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D39" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="F39" s="2" t="s">
+      <c r="E39" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F39" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G39" s="2"/>
-      <c r="H39" s="2"/>
-      <c r="I39" s="2"/>
-      <c r="J39" s="2"/>
-      <c r="K39" s="2"/>
-      <c r="L39" s="2"/>
-      <c r="M39" s="2"/>
-      <c r="N39" s="2"/>
-      <c r="O39" s="2"/>
-      <c r="P39" s="2"/>
-      <c r="Q39" s="2" t="s">
+      <c r="G39" s="3"/>
+      <c r="H39" s="3"/>
+      <c r="I39" s="3"/>
+      <c r="J39" s="3"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="R39" s="2"/>
+      <c r="R39" s="3"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>133</v>
@@ -2949,7 +2954,7 @@
         <v>134</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>218</v>
+        <v>139</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>136</v>
@@ -2970,45 +2975,43 @@
       <c r="R40" s="2"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="2">
-        <v>2</v>
-      </c>
-      <c r="B41" s="2">
-        <v>220</v>
-      </c>
-      <c r="C41" s="2" t="s">
+      <c r="A41" s="3">
+        <v>1</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="C41" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="D41" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E41" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="F41" s="2" t="s">
+      <c r="E41" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G41" s="2"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
-      <c r="O41" s="2"/>
-      <c r="P41" s="2"/>
-      <c r="Q41" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="R41" s="2"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>133</v>
@@ -3017,7 +3020,7 @@
         <v>134</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="F42" s="2" t="s">
         <v>136</v>
@@ -3039,10 +3042,10 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
-        <v>16</v>
-      </c>
-      <c r="B43" s="2">
-        <v>330</v>
+        <v>3</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>144</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>133</v>
@@ -3051,7 +3054,7 @@
         <v>134</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>148</v>
+        <v>217</v>
       </c>
       <c r="F43" s="2" t="s">
         <v>136</v>
@@ -3073,22 +3076,22 @@
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -3100,27 +3103,29 @@
       <c r="N44" s="2"/>
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
-      <c r="Q44" s="2"/>
+      <c r="Q44" s="2" t="s">
+        <v>137</v>
+      </c>
       <c r="R44" s="2"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
@@ -3135,172 +3140,172 @@
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
     </row>
-    <row r="46" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>4</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="G46" s="2"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2"/>
+      <c r="J46" s="2"/>
+      <c r="K46" s="2"/>
+      <c r="L46" s="2"/>
+      <c r="M46" s="2"/>
+      <c r="N46" s="2"/>
+      <c r="O46" s="2"/>
+      <c r="P46" s="2"/>
+      <c r="Q46" s="2"/>
+      <c r="R46" s="2"/>
+    </row>
+    <row r="47" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="3">
         <v>2</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B47" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C46" s="3" t="s">
+      <c r="D47" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="E47" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="F47" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
+      <c r="J47" s="3"/>
+      <c r="K47" s="3"/>
+      <c r="L47" s="3"/>
+      <c r="M47" s="3"/>
+      <c r="N47" s="3"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="3"/>
+      <c r="Q47" s="3"/>
+      <c r="R47" s="3"/>
+    </row>
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>1</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="F46" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3"/>
-      <c r="O46" s="3"/>
-      <c r="P46" s="3"/>
-      <c r="Q46" s="3"/>
-      <c r="R46" s="3"/>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
-        <v>1</v>
-      </c>
-      <c r="B47" s="2" t="s">
+      <c r="C48" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D48" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="D47" s="2" t="s">
+      <c r="E48" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="F48" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="G48" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="H48" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="G47" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="H47" s="2" t="s">
+      <c r="I48" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="I47" s="2" t="s">
+      <c r="J48" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="J47" s="2" t="s">
+      <c r="K48" s="2"/>
+      <c r="L48" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="K47" s="2"/>
-      <c r="L47" s="2" t="s">
+      <c r="M48" s="2"/>
+      <c r="N48" s="2"/>
+      <c r="O48" s="2"/>
+      <c r="P48" s="2"/>
+      <c r="Q48" s="2"/>
+      <c r="R48" s="2"/>
+    </row>
+    <row r="49" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="3">
+        <v>1</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="M47" s="2"/>
-      <c r="N47" s="2"/>
-      <c r="O47" s="2"/>
-      <c r="P47" s="2"/>
-      <c r="Q47" s="2"/>
-      <c r="R47" s="2"/>
-    </row>
-    <row r="48" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3">
-        <v>1</v>
-      </c>
-      <c r="B48" s="3" t="s">
+      <c r="C49" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D48" s="3" t="s">
+      <c r="E49" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="F49" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="G49" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="H49" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="G48" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="H48" s="3" t="s">
+      <c r="I49" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="I48" s="3" t="s">
+      <c r="J49" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="J48" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
-      <c r="O48" s="3"/>
-      <c r="P48" s="3"/>
-      <c r="Q48" s="3"/>
-      <c r="R48" s="3"/>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
-        <v>1</v>
-      </c>
-      <c r="B49" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="F49" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="G49" s="2"/>
-      <c r="H49" s="2"/>
-      <c r="I49" s="2"/>
-      <c r="J49" s="2"/>
-      <c r="K49" s="2"/>
-      <c r="L49" s="2"/>
-      <c r="M49" s="2"/>
-      <c r="N49" s="2"/>
-      <c r="O49" s="2"/>
-      <c r="P49" s="2"/>
-      <c r="Q49" s="2"/>
-      <c r="R49" s="2"/>
+      <c r="M49" s="3"/>
+      <c r="N49" s="3"/>
+      <c r="O49" s="3"/>
+      <c r="P49" s="3"/>
+      <c r="Q49" s="3"/>
+      <c r="R49" s="3"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>1</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C50" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E50" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="F50" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
@@ -3320,19 +3325,19 @@
         <v>1</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -3352,19 +3357,19 @@
         <v>1</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
@@ -3384,19 +3389,19 @@
         <v>1</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
@@ -3416,19 +3421,19 @@
         <v>1</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
@@ -3448,19 +3453,19 @@
         <v>1</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
@@ -3480,19 +3485,19 @@
         <v>1</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
@@ -3512,19 +3517,19 @@
         <v>1</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
@@ -3544,19 +3549,19 @@
         <v>1</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
@@ -3576,19 +3581,19 @@
         <v>1</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
@@ -3608,19 +3613,19 @@
         <v>1</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
@@ -3640,19 +3645,19 @@
         <v>1</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
@@ -3672,19 +3677,19 @@
         <v>1</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
@@ -3704,19 +3709,19 @@
         <v>1</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
@@ -3736,19 +3741,19 @@
         <v>1</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
@@ -3768,19 +3773,19 @@
         <v>1</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
@@ -3800,19 +3805,19 @@
         <v>1</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
@@ -3832,19 +3837,19 @@
         <v>1</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>215</v>
+        <v>176</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>215</v>
+        <v>176</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>217</v>
+        <v>178</v>
       </c>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
@@ -3859,10 +3864,43 @@
       <c r="Q67" s="2"/>
       <c r="R67" s="2"/>
     </row>
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>1</v>
+      </c>
+      <c r="B68" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="G68" s="2"/>
+      <c r="H68" s="2"/>
+      <c r="I68" s="2"/>
+      <c r="J68" s="2"/>
+      <c r="K68" s="2"/>
+      <c r="L68" s="2"/>
+      <c r="M68" s="2"/>
+      <c r="N68" s="2"/>
+      <c r="O68" s="2"/>
+      <c r="P68" s="2"/>
+      <c r="Q68" s="2"/>
+      <c r="R68" s="2"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:R67" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R67">
-      <sortCondition ref="D1:D67"/>
+  <autoFilter ref="A1:R68" xr:uid="{461EE88E-D0F4-4C5C-A3C0-6312330DF6EB}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R68">
+      <sortCondition ref="D2:D68"/>
+      <sortCondition ref="B2:B68"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Checked MIDI input page of schematic
</commit_message>
<xml_diff>
--- a/Hardware/Cornverter BOM 2019 02 09.xlsx
+++ b/Hardware/Cornverter BOM 2019 02 09.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!!Product Design\Cornverter\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA86655-6ACA-4AD2-8F3D-E3091BA3F978}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FCDD98-EEF5-421E-9A40-826D58F4B9CF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1611,8 +1611,8 @@
   <dimension ref="A1:R68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A32" sqref="A32:XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2676,37 +2676,37 @@
       <c r="Q31" s="3"/>
       <c r="R31" s="3"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
-        <v>1</v>
-      </c>
-      <c r="B32" s="2" t="s">
+    <row r="32" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="3">
+        <v>1</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="G32" s="2"/>
-      <c r="H32" s="2"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="2"/>
-      <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
-      <c r="N32" s="2"/>
-      <c r="O32" s="2"/>
-      <c r="P32" s="2"/>
-      <c r="Q32" s="2"/>
-      <c r="R32" s="2"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="3"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
     </row>
     <row r="33" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
@@ -2805,38 +2805,38 @@
       <c r="R35" s="2"/>
     </row>
     <row r="36" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
-        <v>1</v>
-      </c>
-      <c r="B36" s="2">
+      <c r="A36" s="3">
+        <v>1</v>
+      </c>
+      <c r="B36" s="3">
         <v>220</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D36" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E36" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G36" s="2"/>
-      <c r="H36" s="2"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="2"/>
-      <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="2"/>
-      <c r="O36" s="2"/>
-      <c r="P36" s="2"/>
-      <c r="Q36" s="2" t="s">
+      <c r="G36" s="3"/>
+      <c r="H36" s="3"/>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="R36" s="2"/>
+      <c r="R36" s="3"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
@@ -3864,37 +3864,37 @@
       <c r="Q67" s="2"/>
       <c r="R67" s="2"/>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A68" s="2">
-        <v>1</v>
-      </c>
-      <c r="B68" s="2" t="s">
+    <row r="68" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="3">
+        <v>1</v>
+      </c>
+      <c r="B68" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="C68" s="2" t="s">
+      <c r="C68" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="D68" s="2" t="s">
+      <c r="D68" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="E68" s="2" t="s">
+      <c r="E68" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="F68" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="G68" s="2"/>
-      <c r="H68" s="2"/>
-      <c r="I68" s="2"/>
-      <c r="J68" s="2"/>
-      <c r="K68" s="2"/>
-      <c r="L68" s="2"/>
-      <c r="M68" s="2"/>
-      <c r="N68" s="2"/>
-      <c r="O68" s="2"/>
-      <c r="P68" s="2"/>
-      <c r="Q68" s="2"/>
-      <c r="R68" s="2"/>
+      <c r="G68" s="3"/>
+      <c r="H68" s="3"/>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="3"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="3"/>
+      <c r="P68" s="3"/>
+      <c r="Q68" s="3"/>
+      <c r="R68" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:R68" xr:uid="{461EE88E-D0F4-4C5C-A3C0-6312330DF6EB}">

</xml_diff>

<commit_message>
Checked V/oct outs page and happy
</commit_message>
<xml_diff>
--- a/Hardware/Cornverter BOM 2019 02 09.xlsx
+++ b/Hardware/Cornverter BOM 2019 02 09.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!!Product Design\Cornverter\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5FCDD98-EEF5-421E-9A40-826D58F4B9CF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6753E9B6-E129-40EB-8585-F8B113B59278}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="221">
   <si>
     <t>Qty</t>
   </si>
@@ -418,9 +418,6 @@
     <t>Green</t>
   </si>
   <si>
-    <t>LED1, LED2, LED3, LED4, LED5, LED6</t>
-  </si>
-  <si>
     <t>100K</t>
   </si>
   <si>
@@ -454,9 +451,6 @@
     <t>1K</t>
   </si>
   <si>
-    <t>R5, R9, R10, R14, R27, R28, R29, R30, R33, R34, R41, R42, R43, R44, R45, R46, R53, R54, R55, R56, R57, R58</t>
-  </si>
-  <si>
     <t>1M</t>
   </si>
   <si>
@@ -473,9 +467,6 @@
   </si>
   <si>
     <t>SO14</t>
-  </si>
-  <si>
-    <t>IC3, IC4</t>
   </si>
   <si>
     <t>OP AMP</t>
@@ -695,6 +686,78 @@
         <scheme val="minor"/>
       </rPr>
       <t>R35, R36</t>
+    </r>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IC3,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> IC4</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R5, R9, R10, R14,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> R27, R28, R29, R30, R33, R34, R41, R42, R43, R44, R45, R46, R53, R54, R55, R56, R57, R58</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>LED1, LED2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, LED3, LED4, LED5, LED6</t>
     </r>
   </si>
   <si>
@@ -736,7 +799,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">, C9, C10, C11, C20, C21, C24, C25, C27, C28, </t>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>C9, C10, C11,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> C20, C21, C24, C25, C27, C28, </t>
     </r>
     <r>
       <rPr>
@@ -748,12 +831,6 @@
       </rPr>
       <t>C26</t>
     </r>
-  </si>
-  <si>
-    <t>R4</t>
-  </si>
-  <si>
-    <t>R3</t>
   </si>
 </sst>
 </file>
@@ -1611,8 +1688,8 @@
   <dimension ref="A1:R68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32:XFD32"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1902,37 +1979,37 @@
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>1</v>
-      </c>
-      <c r="B9" s="2" t="s">
+    <row r="9" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
@@ -2030,37 +2107,37 @@
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>1</v>
-      </c>
-      <c r="B13" s="2" t="s">
+    <row r="13" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>1</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
@@ -2318,47 +2395,47 @@
       <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+    <row r="22" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
         <v>2</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="F22" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="H22" s="2" t="s">
+      <c r="H22" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="I22" s="2" t="s">
+      <c r="I22" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="J22" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2" t="s">
+      <c r="K22" s="3"/>
+      <c r="L22" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="M22" s="2"/>
-      <c r="N22" s="2"/>
-      <c r="O22" s="2"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="2"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="3"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
@@ -2374,7 +2451,7 @@
         <v>81</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>82</v>
@@ -2786,7 +2863,7 @@
         <v>127</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>131</v>
+        <v>219</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>129</v>
@@ -2812,16 +2889,16 @@
         <v>220</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="E36" s="3" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -2834,7 +2911,7 @@
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
       <c r="Q36" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R36" s="3"/>
     </row>
@@ -2846,16 +2923,16 @@
         <v>280</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="E37" s="2" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -2868,11 +2945,11 @@
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R37" s="2"/>
     </row>
-    <row r="38" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>16</v>
       </c>
@@ -2880,150 +2957,105 @@
         <v>330</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="E38" s="2" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F38" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q38" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="2"/>
-      <c r="L38" s="2"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="2"/>
-      <c r="O38" s="2"/>
-      <c r="P38" s="2"/>
-      <c r="Q38" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="R38" s="2"/>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>2</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="D39" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="F39" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="Q39" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-      <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3" t="s">
+    </row>
+    <row r="40" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>2</v>
+      </c>
+      <c r="B40" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="R39" s="3"/>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
-        <v>2</v>
-      </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="F40" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q40" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>1</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="G40" s="2"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
-      <c r="Q40" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="R40" s="2"/>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" s="3">
-        <v>1</v>
-      </c>
-      <c r="B41" s="3" t="s">
+      <c r="E41" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="F41" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3"/>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3"/>
-      <c r="K41" s="3"/>
-      <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3"/>
-      <c r="O41" s="3"/>
-      <c r="P41" s="3"/>
-      <c r="Q41" s="3"/>
-      <c r="R41" s="3"/>
+        <v>135</v>
+      </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>22</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="E42" s="2" t="s">
-        <v>143</v>
+        <v>218</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
@@ -3036,7 +3068,7 @@
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R42" s="2"/>
     </row>
@@ -3045,19 +3077,19 @@
         <v>3</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C43" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="E43" s="2" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -3070,7 +3102,7 @@
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R43" s="2"/>
     </row>
@@ -3079,19 +3111,19 @@
         <v>8</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C44" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="E44" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -3104,7 +3136,7 @@
       <c r="O44" s="2"/>
       <c r="P44" s="2"/>
       <c r="Q44" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R44" s="2"/>
     </row>
@@ -3113,19 +3145,19 @@
         <v>2</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F45" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>151</v>
       </c>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
@@ -3145,19 +3177,19 @@
         <v>4</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="F46" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>153</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>155</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
@@ -3177,16 +3209,16 @@
         <v>2</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>156</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>159</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>107</v>
@@ -3204,82 +3236,82 @@
       <c r="Q47" s="3"/>
       <c r="R47" s="3"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
-        <v>1</v>
-      </c>
-      <c r="B48" s="2" t="s">
+    <row r="48" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="3">
+        <v>1</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F48" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="G48" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="H48" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="E48" s="2" t="s">
+      <c r="I48" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="J48" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="G48" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="H48" s="2" t="s">
+      <c r="K48" s="3"/>
+      <c r="L48" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="I48" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="K48" s="2"/>
-      <c r="L48" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="M48" s="2"/>
-      <c r="N48" s="2"/>
-      <c r="O48" s="2"/>
-      <c r="P48" s="2"/>
-      <c r="Q48" s="2"/>
-      <c r="R48" s="2"/>
+      <c r="M48" s="3"/>
+      <c r="N48" s="3"/>
+      <c r="O48" s="3"/>
+      <c r="P48" s="3"/>
+      <c r="Q48" s="3"/>
+      <c r="R48" s="3"/>
     </row>
     <row r="49" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>1</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F49" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="G49" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="H49" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="I49" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="F49" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>171</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>173</v>
-      </c>
       <c r="J49" s="3" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="K49" s="3"/>
       <c r="L49" s="3" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
@@ -3293,19 +3325,19 @@
         <v>1</v>
       </c>
       <c r="B50" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="F50" s="2" t="s">
-        <v>178</v>
       </c>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
@@ -3325,19 +3357,19 @@
         <v>1</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -3357,19 +3389,19 @@
         <v>1</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
@@ -3389,19 +3421,19 @@
         <v>1</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
@@ -3421,19 +3453,19 @@
         <v>1</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
@@ -3453,19 +3485,19 @@
         <v>1</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
@@ -3480,56 +3512,56 @@
       <c r="Q55" s="2"/>
       <c r="R55" s="2"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A56" s="2">
-        <v>1</v>
-      </c>
-      <c r="B56" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="F56" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="G56" s="2"/>
-      <c r="H56" s="2"/>
-      <c r="I56" s="2"/>
-      <c r="J56" s="2"/>
-      <c r="K56" s="2"/>
-      <c r="L56" s="2"/>
-      <c r="M56" s="2"/>
-      <c r="N56" s="2"/>
-      <c r="O56" s="2"/>
-      <c r="P56" s="2"/>
-      <c r="Q56" s="2"/>
-      <c r="R56" s="2"/>
+    <row r="56" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>1</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="3"/>
+      <c r="O56" s="3"/>
+      <c r="P56" s="3"/>
+      <c r="Q56" s="3"/>
+      <c r="R56" s="3"/>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>1</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
@@ -3549,19 +3581,19 @@
         <v>1</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
@@ -3581,19 +3613,19 @@
         <v>1</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
@@ -3613,19 +3645,19 @@
         <v>1</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
@@ -3645,19 +3677,19 @@
         <v>1</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
@@ -3677,19 +3709,19 @@
         <v>1</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
@@ -3709,19 +3741,19 @@
         <v>1</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
@@ -3736,56 +3768,56 @@
       <c r="Q63" s="2"/>
       <c r="R63" s="2"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A64" s="2">
-        <v>1</v>
-      </c>
-      <c r="B64" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>178</v>
-      </c>
-      <c r="G64" s="2"/>
-      <c r="H64" s="2"/>
-      <c r="I64" s="2"/>
-      <c r="J64" s="2"/>
-      <c r="K64" s="2"/>
-      <c r="L64" s="2"/>
-      <c r="M64" s="2"/>
-      <c r="N64" s="2"/>
-      <c r="O64" s="2"/>
-      <c r="P64" s="2"/>
-      <c r="Q64" s="2"/>
-      <c r="R64" s="2"/>
+    <row r="64" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="3">
+        <v>1</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
+      <c r="J64" s="3"/>
+      <c r="K64" s="3"/>
+      <c r="L64" s="3"/>
+      <c r="M64" s="3"/>
+      <c r="N64" s="3"/>
+      <c r="O64" s="3"/>
+      <c r="P64" s="3"/>
+      <c r="Q64" s="3"/>
+      <c r="R64" s="3"/>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>1</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
@@ -3805,19 +3837,19 @@
         <v>1</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
@@ -3837,19 +3869,19 @@
         <v>1</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
@@ -3869,19 +3901,19 @@
         <v>1</v>
       </c>
       <c r="B68" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D68" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="E68" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F68" s="3" t="s">
         <v>213</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>214</v>
-      </c>
-      <c r="E68" s="3" t="s">
-        <v>215</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>216</v>
       </c>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>

</xml_diff>

<commit_message>
Checked over schematic sheet 3 PWM outputs
</commit_message>
<xml_diff>
--- a/Hardware/Cornverter BOM 2019 02 09.xlsx
+++ b/Hardware/Cornverter BOM 2019 02 09.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!!Product Design\Cornverter\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6753E9B6-E129-40EB-8585-F8B113B59278}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF3F068-77EF-4C50-BE78-4A56B12DA2D2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -418,6 +418,9 @@
     <t>Green</t>
   </si>
   <si>
+    <t>LED1, LED2, LED3, LED4, LED5, LED6</t>
+  </si>
+  <si>
     <t>100K</t>
   </si>
   <si>
@@ -460,15 +463,15 @@
     <t>R19, R20, R21, R22, R23, R24, R25, R26</t>
   </si>
   <si>
-    <t>R15, R16, R17, R18, R31, R32, R37, R38, R39, R40, R47, R48, R49, R50, R51, R52</t>
-  </si>
-  <si>
     <t>TL074D</t>
   </si>
   <si>
     <t>SO14</t>
   </si>
   <si>
+    <t>IC3, IC4</t>
+  </si>
+  <si>
     <t>OP AMP</t>
   </si>
   <si>
@@ -476,9 +479,6 @@
   </si>
   <si>
     <t>SO16</t>
-  </si>
-  <si>
-    <t>IC5, IC6, IC7, IC8</t>
   </si>
   <si>
     <t>Hex non-inverting BUFFER</t>
@@ -693,72 +693,6 @@
   </si>
   <si>
     <t>R3</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>IC3,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> IC4</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>R5, R9, R10, R14,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> R27, R28, R29, R30, R33, R34, R41, R42, R43, R44, R45, R46, R53, R54, R55, R56, R57, R58</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>LED1, LED2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, LED3, LED4, LED5, LED6</t>
-    </r>
   </si>
   <si>
     <r>
@@ -809,7 +743,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>C9, C10, C11,</t>
+      <t>C9, C10, C11, C20, C21</t>
     </r>
     <r>
       <rPr>
@@ -819,7 +753,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> C20, C21, C24, C25, C27, C28, </t>
+      <t xml:space="preserve">, C24, C25, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">C27, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">C28, </t>
     </r>
     <r>
       <rPr>
@@ -830,6 +784,75 @@
         <scheme val="minor"/>
       </rPr>
       <t>C26</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R5, R9, R10, R14, R27, R28, R29, R30</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, R33, R34, R41, R42, R43, R44, R45, R46, R53, R54, R55, R56, R57, R58</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>IC5, IC6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, IC7, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IC8</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R15, R16, R17, R18,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> R31, R32, R37, R38, R39, R40, R47, R48, R49, R50, R51, R52</t>
     </r>
   </si>
 </sst>
@@ -1688,8 +1711,8 @@
   <dimension ref="A1:R68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E24" sqref="E24"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35:XFD35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1883,69 +1906,69 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>1</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+    </row>
+    <row r="7" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>1</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
@@ -2011,69 +2034,69 @@
       <c r="Q9" s="3"/>
       <c r="R9" s="3"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>1</v>
-      </c>
-      <c r="B10" s="2" t="s">
+    <row r="10" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>1</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+    </row>
+    <row r="11" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>1</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -2451,7 +2474,7 @@
         <v>81</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>82</v>
@@ -2471,39 +2494,39 @@
       </c>
       <c r="R23" s="2"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+    <row r="24" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
         <v>8</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
-      <c r="N24" s="2"/>
-      <c r="O24" s="2"/>
-      <c r="P24" s="2"/>
-      <c r="Q24" s="2" t="s">
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="3"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="R24" s="2"/>
+      <c r="R24" s="3"/>
     </row>
     <row r="25" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
@@ -2849,37 +2872,37 @@
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+    <row r="35" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
         <v>6</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="F35" s="2" t="s">
+      <c r="E35" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="G35" s="2"/>
-      <c r="H35" s="2"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="2"/>
-      <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="2"/>
-      <c r="O35" s="2"/>
-      <c r="P35" s="2"/>
-      <c r="Q35" s="2"/>
-      <c r="R35" s="2"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3"/>
+      <c r="I35" s="3"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
+      <c r="N35" s="3"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
     </row>
     <row r="36" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
@@ -2889,16 +2912,16 @@
         <v>220</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>215</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -2911,7 +2934,7 @@
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
       <c r="Q36" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="R36" s="3"/>
     </row>
@@ -2923,16 +2946,16 @@
         <v>280</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>216</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -2945,7 +2968,7 @@
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="R37" s="2"/>
     </row>
@@ -2957,19 +2980,19 @@
         <v>330</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>145</v>
+        <v>220</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Q38" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2977,22 +3000,22 @@
         <v>2</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Q39" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3000,22 +3023,22 @@
         <v>2</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q40" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q40" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3023,19 +3046,19 @@
         <v>1</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
@@ -3043,19 +3066,19 @@
         <v>22</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>218</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
@@ -3068,7 +3091,7 @@
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="2" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="R42" s="2"/>
     </row>
@@ -3077,19 +3100,19 @@
         <v>3</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E43" s="2" t="s">
         <v>214</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
@@ -3102,91 +3125,91 @@
       <c r="O43" s="2"/>
       <c r="P43" s="2"/>
       <c r="Q43" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="R43" s="2"/>
+    </row>
+    <row r="44" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>8</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="F44" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="R43" s="2"/>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" s="2">
-        <v>8</v>
-      </c>
-      <c r="B44" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="F44" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="G44" s="2"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
-      <c r="O44" s="2"/>
-      <c r="P44" s="2"/>
-      <c r="Q44" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="R44" s="2"/>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" s="2">
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="3"/>
+      <c r="Q44" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="R44" s="3"/>
+    </row>
+    <row r="45" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
         <v>2</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F45" s="2" t="s">
+      <c r="E45" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="G45" s="2"/>
-      <c r="H45" s="2"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="2"/>
-      <c r="L45" s="2"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="2"/>
-      <c r="O45" s="2"/>
-      <c r="P45" s="2"/>
-      <c r="Q45" s="2"/>
-      <c r="R45" s="2"/>
+      <c r="F45" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="K45" s="3"/>
+      <c r="L45" s="3"/>
+      <c r="M45" s="3"/>
+      <c r="N45" s="3"/>
+      <c r="O45" s="3"/>
+      <c r="P45" s="3"/>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="3"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>4</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>151</v>
+        <v>219</v>
       </c>
       <c r="F46" s="2" t="s">
         <v>152</v>
@@ -3320,69 +3343,69 @@
       <c r="Q49" s="3"/>
       <c r="R49" s="3"/>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
-        <v>1</v>
-      </c>
-      <c r="B50" s="2" t="s">
+    <row r="50" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="3">
+        <v>1</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C50" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="D50" s="2" t="s">
+      <c r="D50" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E50" s="2" t="s">
+      <c r="E50" s="3" t="s">
         <v>174</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="F50" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="G50" s="2"/>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="2"/>
-      <c r="L50" s="2"/>
-      <c r="M50" s="2"/>
-      <c r="N50" s="2"/>
-      <c r="O50" s="2"/>
-      <c r="P50" s="2"/>
-      <c r="Q50" s="2"/>
-      <c r="R50" s="2"/>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
-        <v>1</v>
-      </c>
-      <c r="B51" s="2" t="s">
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
+      <c r="N50" s="3"/>
+      <c r="O50" s="3"/>
+      <c r="P50" s="3"/>
+      <c r="Q50" s="3"/>
+      <c r="R50" s="3"/>
+    </row>
+    <row r="51" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="3">
+        <v>1</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="D51" s="2" t="s">
+      <c r="D51" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="E51" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="F51" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
-      <c r="L51" s="2"/>
-      <c r="M51" s="2"/>
-      <c r="N51" s="2"/>
-      <c r="O51" s="2"/>
-      <c r="P51" s="2"/>
-      <c r="Q51" s="2"/>
-      <c r="R51" s="2"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="O51" s="3"/>
+      <c r="P51" s="3"/>
+      <c r="Q51" s="3"/>
+      <c r="R51" s="3"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
@@ -3576,69 +3599,69 @@
       <c r="Q57" s="2"/>
       <c r="R57" s="2"/>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A58" s="2">
-        <v>1</v>
-      </c>
-      <c r="B58" s="2" t="s">
+    <row r="58" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>1</v>
+      </c>
+      <c r="B58" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C58" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D58" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E58" s="2" t="s">
+      <c r="E58" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="F58" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="G58" s="2"/>
-      <c r="H58" s="2"/>
-      <c r="I58" s="2"/>
-      <c r="J58" s="2"/>
-      <c r="K58" s="2"/>
-      <c r="L58" s="2"/>
-      <c r="M58" s="2"/>
-      <c r="N58" s="2"/>
-      <c r="O58" s="2"/>
-      <c r="P58" s="2"/>
-      <c r="Q58" s="2"/>
-      <c r="R58" s="2"/>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A59" s="2">
-        <v>1</v>
-      </c>
-      <c r="B59" s="2" t="s">
+      <c r="G58" s="3"/>
+      <c r="H58" s="3"/>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="3"/>
+      <c r="N58" s="3"/>
+      <c r="O58" s="3"/>
+      <c r="P58" s="3"/>
+      <c r="Q58" s="3"/>
+      <c r="R58" s="3"/>
+    </row>
+    <row r="59" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
+        <v>1</v>
+      </c>
+      <c r="B59" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="C59" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="D59" s="2" t="s">
+      <c r="D59" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="E59" s="2" t="s">
+      <c r="E59" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="F59" s="2" t="s">
+      <c r="F59" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="G59" s="2"/>
-      <c r="H59" s="2"/>
-      <c r="I59" s="2"/>
-      <c r="J59" s="2"/>
-      <c r="K59" s="2"/>
-      <c r="L59" s="2"/>
-      <c r="M59" s="2"/>
-      <c r="N59" s="2"/>
-      <c r="O59" s="2"/>
-      <c r="P59" s="2"/>
-      <c r="Q59" s="2"/>
-      <c r="R59" s="2"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="3"/>
+      <c r="I59" s="3"/>
+      <c r="J59" s="3"/>
+      <c r="K59" s="3"/>
+      <c r="L59" s="3"/>
+      <c r="M59" s="3"/>
+      <c r="N59" s="3"/>
+      <c r="O59" s="3"/>
+      <c r="P59" s="3"/>
+      <c r="Q59" s="3"/>
+      <c r="R59" s="3"/>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="2">

</xml_diff>

<commit_message>
Checked PWM Outputs page of schematic
</commit_message>
<xml_diff>
--- a/Hardware/Cornverter BOM 2019 02 09.xlsx
+++ b/Hardware/Cornverter BOM 2019 02 09.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!!Product Design\Cornverter\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF3F068-77EF-4C50-BE78-4A56B12DA2D2}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20BD0D6-17FD-4DEE-A179-917306F1896D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="221">
   <si>
     <t>Qty</t>
   </si>
@@ -343,9 +343,6 @@
     <t>DO35-7</t>
   </si>
   <si>
-    <t>D3, D4, D5</t>
-  </si>
-  <si>
     <t>DIODE</t>
   </si>
   <si>
@@ -665,28 +662,6 @@
   </si>
   <si>
     <t>Thonkiconn stereo jack</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">R2, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>R35, R36</t>
-    </r>
   </si>
   <si>
     <t>R4</t>
@@ -743,7 +718,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>C9, C10, C11, C20, C21</t>
+      <t xml:space="preserve">C9, C10, C11, C20, C21, C24, </t>
     </r>
     <r>
       <rPr>
@@ -753,7 +728,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">, C24, C25, </t>
+      <t xml:space="preserve">C25, </t>
     </r>
     <r>
       <rPr>
@@ -763,7 +738,19 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">C27, </t>
+      <t>C27, C28, C26</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>IC5,</t>
     </r>
     <r>
       <rPr>
@@ -773,7 +760,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">C28, </t>
+      <t xml:space="preserve"> IC6</t>
     </r>
     <r>
       <rPr>
@@ -783,10 +770,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>C26</t>
+      <t>, IC7, IC8</t>
     </r>
   </si>
   <si>
+    <r>
+      <t>D3,</t>
+    </r>
     <r>
       <rPr>
         <sz val="11"/>
@@ -795,7 +785,19 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>R5, R9, R10, R14, R27, R28, R29, R30</t>
+      <t xml:space="preserve"> D4, D5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="9" tint="-0.249977111117893"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>R5, R9, R10, R14, R27, R28, R29, R30, R33, R34, R41, R42, R43, R44, R45, R46,</t>
     </r>
     <r>
       <rPr>
@@ -805,13 +807,13 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, R33, R34, R41, R42, R43, R44, R45, R46, R53, R54, R55, R56, R57, R58</t>
+      <t xml:space="preserve"> R53, R54, R55, R56, R57, R58</t>
     </r>
   </si>
   <si>
-    <r>
-      <t>IC5, IC6</t>
-    </r>
+    <t>R2, R35, R36</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -820,7 +822,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">, IC7, </t>
+      <t>R15, R16, R17, R18, R31, R32, R37, R38, R39, R40,</t>
     </r>
     <r>
       <rPr>
@@ -830,29 +832,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>IC8</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>R15, R16, R17, R18,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> R31, R32, R37, R38, R39, R40, R47, R48, R49, R50, R51, R52</t>
+      <t xml:space="preserve"> R47, R48, R49, R50, R51, R52</t>
     </r>
   </si>
 </sst>
@@ -1711,8 +1691,8 @@
   <dimension ref="A1:R68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A35" sqref="A35:XFD35"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1810,37 +1790,37 @@
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>1</v>
-      </c>
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
     </row>
     <row r="4" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -1874,37 +1854,37 @@
       <c r="Q4" s="3"/>
       <c r="R4" s="3"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
     </row>
     <row r="6" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -1970,37 +1950,37 @@
       <c r="Q7" s="3"/>
       <c r="R7" s="3"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>1</v>
-      </c>
-      <c r="B8" s="2" t="s">
+    <row r="8" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
     </row>
     <row r="9" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
@@ -2098,37 +2078,37 @@
       <c r="Q11" s="3"/>
       <c r="R11" s="3"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>1</v>
-      </c>
-      <c r="B12" s="2" t="s">
+    <row r="12" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="2"/>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
     </row>
     <row r="13" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
@@ -2162,69 +2142,69 @@
       <c r="Q13" s="3"/>
       <c r="R13" s="3"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>1</v>
-      </c>
-      <c r="B14" s="2" t="s">
+    <row r="14" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>1</v>
-      </c>
-      <c r="B15" s="2" t="s">
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+    </row>
+    <row r="15" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="F15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -2474,7 +2454,7 @@
         <v>81</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>82</v>
@@ -2562,39 +2542,39 @@
       </c>
       <c r="R25" s="3"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+    <row r="26" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
         <v>2</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
-      <c r="P26" s="2"/>
-      <c r="Q26" s="2" t="s">
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="3"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="R26" s="2"/>
+      <c r="R26" s="3"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
@@ -2688,10 +2668,10 @@
         <v>105</v>
       </c>
       <c r="E29" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
@@ -2711,19 +2691,19 @@
         <v>3</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="F30" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -2745,19 +2725,19 @@
         <v>1</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>116</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>117</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -2770,7 +2750,7 @@
         <v>1667008</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
@@ -2781,19 +2761,19 @@
         <v>1</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>119</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>120</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>66</v>
       </c>
       <c r="E32" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="F32" s="3" t="s">
-        <v>122</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -2813,19 +2793,19 @@
         <v>1</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D33" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>125</v>
-      </c>
       <c r="F33" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -2845,19 +2825,19 @@
         <v>12</v>
       </c>
       <c r="B34" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C34" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E34" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E34" s="2" t="s">
+      <c r="F34" s="2" t="s">
         <v>128</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>129</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -2877,19 +2857,19 @@
         <v>6</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>131</v>
-      </c>
       <c r="F35" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -2912,16 +2892,16 @@
         <v>220</v>
       </c>
       <c r="C36" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D36" s="3" t="s">
-        <v>134</v>
-      </c>
       <c r="E36" s="3" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -2934,7 +2914,7 @@
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
       <c r="Q36" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R36" s="3"/>
     </row>
@@ -2946,16 +2926,16 @@
         <v>280</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="E37" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
@@ -2968,7 +2948,7 @@
       <c r="O37" s="2"/>
       <c r="P37" s="2"/>
       <c r="Q37" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R37" s="2"/>
     </row>
@@ -2980,19 +2960,19 @@
         <v>330</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="E38" s="2" t="s">
         <v>220</v>
       </c>
       <c r="F38" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q38" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="Q38" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3000,22 +2980,22 @@
         <v>2</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C39" s="3" t="s">
+      <c r="D39" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="E39" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="F39" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="Q39" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="Q39" s="3" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3023,22 +3003,22 @@
         <v>2</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="F40" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q40" s="3" t="s">
         <v>136</v>
-      </c>
-      <c r="Q40" s="3" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="41" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3046,19 +3026,19 @@
         <v>1</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="F41" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
@@ -3066,19 +3046,19 @@
         <v>22</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>134</v>
       </c>
       <c r="E42" s="2" t="s">
         <v>218</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
@@ -3091,62 +3071,62 @@
       <c r="O42" s="2"/>
       <c r="P42" s="2"/>
       <c r="Q42" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R42" s="2"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" s="2">
+    <row r="43" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
         <v>3</v>
       </c>
-      <c r="B43" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="C43" s="2" t="s">
+      <c r="B43" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="F43" s="2" t="s">
+      <c r="E43" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="K43" s="3"/>
+      <c r="L43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="G43" s="2"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
-      <c r="O43" s="2"/>
-      <c r="P43" s="2"/>
-      <c r="Q43" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="R43" s="2"/>
+      <c r="R43" s="3"/>
     </row>
     <row r="44" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>8</v>
       </c>
       <c r="B44" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>134</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>145</v>
-      </c>
       <c r="F44" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -3159,7 +3139,7 @@
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
       <c r="Q44" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="R44" s="3"/>
     </row>
@@ -3168,19 +3148,19 @@
         <v>2</v>
       </c>
       <c r="B45" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="D45" s="3" t="s">
+      <c r="E45" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="F45" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="F45" s="3" t="s">
-        <v>149</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -3200,19 +3180,19 @@
         <v>4</v>
       </c>
       <c r="B46" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D46" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C46" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D46" s="2" t="s">
+      <c r="E46" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="F46" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>152</v>
       </c>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
@@ -3232,19 +3212,19 @@
         <v>2</v>
       </c>
       <c r="B47" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C47" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="D47" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="E47" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>156</v>
-      </c>
       <c r="F47" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
@@ -3264,35 +3244,35 @@
         <v>1</v>
       </c>
       <c r="B48" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D48" s="3" t="s">
+      <c r="E48" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="F48" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="G48" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="H48" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="G48" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="H48" s="3" t="s">
+      <c r="I48" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="I48" s="3" t="s">
+      <c r="J48" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="J48" s="3" t="s">
-        <v>163</v>
       </c>
       <c r="K48" s="3"/>
       <c r="L48" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="M48" s="3"/>
       <c r="N48" s="3"/>
@@ -3306,35 +3286,35 @@
         <v>1</v>
       </c>
       <c r="B49" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>165</v>
-      </c>
-      <c r="D49" s="3" t="s">
+      <c r="E49" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="E49" s="3" t="s">
+      <c r="F49" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="G49" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="H49" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="G49" s="3" t="s">
-        <v>168</v>
-      </c>
-      <c r="H49" s="3" t="s">
+      <c r="I49" s="3" t="s">
         <v>169</v>
       </c>
-      <c r="I49" s="3" t="s">
-        <v>170</v>
-      </c>
       <c r="J49" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="K49" s="3"/>
       <c r="L49" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
@@ -3348,19 +3328,19 @@
         <v>1</v>
       </c>
       <c r="B50" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="D50" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="D50" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="E50" s="3" t="s">
+      <c r="F50" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="F50" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
@@ -3380,19 +3360,19 @@
         <v>1</v>
       </c>
       <c r="B51" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E51" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="C51" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="E51" s="3" t="s">
-        <v>177</v>
-      </c>
       <c r="F51" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
@@ -3412,19 +3392,19 @@
         <v>1</v>
       </c>
       <c r="B52" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E52" s="2" t="s">
         <v>178</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>179</v>
-      </c>
       <c r="F52" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
@@ -3444,19 +3424,19 @@
         <v>1</v>
       </c>
       <c r="B53" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E53" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>181</v>
-      </c>
       <c r="F53" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
@@ -3476,19 +3456,19 @@
         <v>1</v>
       </c>
       <c r="B54" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E54" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>183</v>
-      </c>
       <c r="F54" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
@@ -3508,19 +3488,19 @@
         <v>1</v>
       </c>
       <c r="B55" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E55" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>185</v>
-      </c>
       <c r="F55" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
@@ -3540,19 +3520,19 @@
         <v>1</v>
       </c>
       <c r="B56" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E56" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="C56" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>187</v>
-      </c>
       <c r="F56" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
@@ -3572,19 +3552,19 @@
         <v>1</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E57" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>189</v>
-      </c>
       <c r="F57" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
@@ -3604,19 +3584,19 @@
         <v>1</v>
       </c>
       <c r="B58" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E58" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="C58" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>191</v>
-      </c>
       <c r="F58" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
@@ -3636,19 +3616,19 @@
         <v>1</v>
       </c>
       <c r="B59" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D59" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="C59" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>193</v>
-      </c>
       <c r="F59" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
@@ -3668,19 +3648,19 @@
         <v>1</v>
       </c>
       <c r="B60" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E60" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C60" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>195</v>
-      </c>
       <c r="F60" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
@@ -3695,120 +3675,120 @@
       <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A61" s="2">
-        <v>1</v>
-      </c>
-      <c r="B61" s="2" t="s">
+    <row r="61" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>1</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E61" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="C61" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E61" s="2" t="s">
+      <c r="F61" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
+      <c r="J61" s="3"/>
+      <c r="K61" s="3"/>
+      <c r="L61" s="3"/>
+      <c r="M61" s="3"/>
+      <c r="N61" s="3"/>
+      <c r="O61" s="3"/>
+      <c r="P61" s="3"/>
+      <c r="Q61" s="3"/>
+      <c r="R61" s="3"/>
+    </row>
+    <row r="62" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <v>1</v>
+      </c>
+      <c r="B62" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="F61" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
-      <c r="L61" s="2"/>
-      <c r="M61" s="2"/>
-      <c r="N61" s="2"/>
-      <c r="O61" s="2"/>
-      <c r="P61" s="2"/>
-      <c r="Q61" s="2"/>
-      <c r="R61" s="2"/>
-    </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A62" s="2">
-        <v>1</v>
-      </c>
-      <c r="B62" s="2" t="s">
+      <c r="C62" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E62" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E62" s="2" t="s">
+      <c r="F62" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="3"/>
+      <c r="N62" s="3"/>
+      <c r="O62" s="3"/>
+      <c r="P62" s="3"/>
+      <c r="Q62" s="3"/>
+      <c r="R62" s="3"/>
+    </row>
+    <row r="63" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <v>1</v>
+      </c>
+      <c r="B63" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="F62" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="G62" s="2"/>
-      <c r="H62" s="2"/>
-      <c r="I62" s="2"/>
-      <c r="J62" s="2"/>
-      <c r="K62" s="2"/>
-      <c r="L62" s="2"/>
-      <c r="M62" s="2"/>
-      <c r="N62" s="2"/>
-      <c r="O62" s="2"/>
-      <c r="P62" s="2"/>
-      <c r="Q62" s="2"/>
-      <c r="R62" s="2"/>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A63" s="2">
-        <v>1</v>
-      </c>
-      <c r="B63" s="2" t="s">
+      <c r="C63" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E63" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="C63" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="G63" s="2"/>
-      <c r="H63" s="2"/>
-      <c r="I63" s="2"/>
-      <c r="J63" s="2"/>
-      <c r="K63" s="2"/>
-      <c r="L63" s="2"/>
-      <c r="M63" s="2"/>
-      <c r="N63" s="2"/>
-      <c r="O63" s="2"/>
-      <c r="P63" s="2"/>
-      <c r="Q63" s="2"/>
-      <c r="R63" s="2"/>
+      <c r="F63" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
+      <c r="J63" s="3"/>
+      <c r="K63" s="3"/>
+      <c r="L63" s="3"/>
+      <c r="M63" s="3"/>
+      <c r="N63" s="3"/>
+      <c r="O63" s="3"/>
+      <c r="P63" s="3"/>
+      <c r="Q63" s="3"/>
+      <c r="R63" s="3"/>
     </row>
     <row r="64" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>1</v>
       </c>
       <c r="B64" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E64" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="C64" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="E64" s="3" t="s">
-        <v>203</v>
-      </c>
       <c r="F64" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
@@ -3823,56 +3803,56 @@
       <c r="Q64" s="3"/>
       <c r="R64" s="3"/>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A65" s="2">
-        <v>1</v>
-      </c>
-      <c r="B65" s="2" t="s">
+    <row r="65" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="3">
+        <v>1</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="E65" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="F65" s="2" t="s">
-        <v>175</v>
-      </c>
-      <c r="G65" s="2"/>
-      <c r="H65" s="2"/>
-      <c r="I65" s="2"/>
-      <c r="J65" s="2"/>
-      <c r="K65" s="2"/>
-      <c r="L65" s="2"/>
-      <c r="M65" s="2"/>
-      <c r="N65" s="2"/>
-      <c r="O65" s="2"/>
-      <c r="P65" s="2"/>
-      <c r="Q65" s="2"/>
-      <c r="R65" s="2"/>
+      <c r="F65" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
+      <c r="J65" s="3"/>
+      <c r="K65" s="3"/>
+      <c r="L65" s="3"/>
+      <c r="M65" s="3"/>
+      <c r="N65" s="3"/>
+      <c r="O65" s="3"/>
+      <c r="P65" s="3"/>
+      <c r="Q65" s="3"/>
+      <c r="R65" s="3"/>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>1</v>
       </c>
       <c r="B66" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E66" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>207</v>
-      </c>
       <c r="F66" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
@@ -3892,19 +3872,19 @@
         <v>1</v>
       </c>
       <c r="B67" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C67" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E67" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="C67" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>173</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>209</v>
-      </c>
       <c r="F67" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
@@ -3924,19 +3904,19 @@
         <v>1</v>
       </c>
       <c r="B68" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C68" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="C68" s="3" t="s">
+      <c r="D68" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="E68" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="D68" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="E68" s="3" t="s">
+      <c r="F68" s="3" t="s">
         <v>212</v>
-      </c>
-      <c r="F68" s="3" t="s">
-        <v>213</v>
       </c>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>

</xml_diff>

<commit_message>
Finished checking entire schematic for design errors
</commit_message>
<xml_diff>
--- a/Hardware/Cornverter BOM 2019 02 09.xlsx
+++ b/Hardware/Cornverter BOM 2019 02 09.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\!!Product Design\Cornverter\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F20BD0D6-17FD-4DEE-A179-917306F1896D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32A4DAB0-17BB-4FE7-A1B3-1E285307C566}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -343,6 +343,9 @@
     <t>DO35-7</t>
   </si>
   <si>
+    <t>D3, D4, D5</t>
+  </si>
+  <si>
     <t>DIODE</t>
   </si>
   <si>
@@ -451,6 +454,9 @@
     <t>1K</t>
   </si>
   <si>
+    <t>R5, R9, R10, R14, R27, R28, R29, R30, R33, R34, R41, R42, R43, R44, R45, R46, R53, R54, R55, R56, R57, R58</t>
+  </si>
+  <si>
     <t>1M</t>
   </si>
   <si>
@@ -460,6 +466,9 @@
     <t>R19, R20, R21, R22, R23, R24, R25, R26</t>
   </si>
   <si>
+    <t>R15, R16, R17, R18, R31, R32, R37, R38, R39, R40, R47, R48, R49, R50, R51, R52</t>
+  </si>
+  <si>
     <t>TL074D</t>
   </si>
   <si>
@@ -478,6 +487,9 @@
     <t>SO16</t>
   </si>
   <si>
+    <t>IC5, IC6, IC7, IC8</t>
+  </si>
+  <si>
     <t>Hex non-inverting BUFFER</t>
   </si>
   <si>
@@ -670,177 +682,17 @@
     <t>R3</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C1,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C6, C7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">C9, C10, C11, C20, C21, C24, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">C25, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>C27, C28, C26</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>IC5,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> IC6</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, IC7, IC8</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>D3,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> D4, D5</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>R5, R9, R10, R14, R27, R28, R29, R30, R33, R34, R41, R42, R43, R44, R45, R46,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> R53, R54, R55, R56, R57, R58</t>
-    </r>
-  </si>
-  <si>
     <t>R2, R35, R36</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="9" tint="-0.249977111117893"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>R15, R16, R17, R18, R31, R32, R37, R38, R39, R40,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> R47, R48, R49, R50, R51, R52</t>
-    </r>
+    <t>C1, C6, C7, C9, C10, C11, C20, C21, C24, C25, C27, C28, C26</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -971,13 +823,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="9" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1691,8 +1536,8 @@
   <dimension ref="A1:R68"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K28" sqref="K28"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2206,133 +2051,133 @@
       <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>1</v>
-      </c>
-      <c r="B16" s="2" t="s">
+    <row r="16" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>1</v>
-      </c>
-      <c r="B17" s="2" t="s">
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="3"/>
+    </row>
+    <row r="17" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="F17" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="2"/>
-      <c r="O17" s="2"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>1</v>
-      </c>
-      <c r="B18" s="2" t="s">
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+    </row>
+    <row r="18" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="2"/>
-      <c r="O18" s="2"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>1</v>
-      </c>
-      <c r="B19" s="2" t="s">
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="3"/>
+    </row>
+    <row r="19" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>1</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="2"/>
-      <c r="O19" s="2"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="3"/>
     </row>
     <row r="20" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
@@ -2440,39 +2285,39 @@
       <c r="Q22" s="3"/>
       <c r="R22" s="3"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+    <row r="23" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
         <v>13</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E23" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="F23" s="2" t="s">
+      <c r="E23" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="F23" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="2"/>
-      <c r="O23" s="2"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="2" t="s">
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="3"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="R23" s="2"/>
+      <c r="R23" s="3"/>
     </row>
     <row r="24" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
@@ -2576,47 +2421,47 @@
       </c>
       <c r="R26" s="3"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>1</v>
-      </c>
-      <c r="B27" s="2" t="s">
+    <row r="27" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>1</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C27" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D27" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="E27" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2" t="s">
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="L27" s="2"/>
-      <c r="M27" s="2" t="s">
+      <c r="L27" s="3"/>
+      <c r="M27" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="N27" s="2">
+      <c r="N27" s="3">
         <v>9860150</v>
       </c>
-      <c r="O27" s="2" t="s">
+      <c r="O27" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="P27" s="2"/>
-      <c r="Q27" s="2" t="s">
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="R27" s="2"/>
+      <c r="R27" s="3"/>
     </row>
     <row r="28" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
@@ -2654,56 +2499,56 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+    <row r="29" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
         <v>3</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F29" s="2" t="s">
+      <c r="E29" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
-      <c r="R29" s="2"/>
+      <c r="F29" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
     </row>
     <row r="30" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>3</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
@@ -2725,19 +2570,19 @@
         <v>1</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
@@ -2750,7 +2595,7 @@
         <v>1667008</v>
       </c>
       <c r="O31" s="3" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="P31" s="3"/>
       <c r="Q31" s="3"/>
@@ -2761,19 +2606,19 @@
         <v>1</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>66</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
@@ -2793,19 +2638,19 @@
         <v>1</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F33" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="F33" s="3" t="s">
-        <v>121</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
@@ -2820,56 +2665,56 @@
       <c r="Q33" s="3"/>
       <c r="R33" s="3"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+    <row r="34" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="3">
         <v>12</v>
       </c>
-      <c r="B34" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C34" s="2" t="s">
+      <c r="B34" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="E34" s="2" t="s">
+      <c r="C34" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="D34" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="G34" s="2"/>
-      <c r="H34" s="2"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="2"/>
-      <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="2"/>
-      <c r="O34" s="2"/>
-      <c r="P34" s="2"/>
-      <c r="Q34" s="2"/>
-      <c r="R34" s="2"/>
+      <c r="F34" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3"/>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
     </row>
     <row r="35" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>6</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>129</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>128</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
@@ -2892,16 +2737,16 @@
         <v>220</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>213</v>
+        <v>217</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G36" s="3"/>
       <c r="H36" s="3"/>
@@ -2914,65 +2759,65 @@
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
       <c r="Q36" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="R36" s="3"/>
+    </row>
+    <row r="37" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>1</v>
+      </c>
+      <c r="B37" s="3">
+        <v>280</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="R36" s="3"/>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <v>1</v>
-      </c>
-      <c r="B37" s="2">
-        <v>280</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D37" s="2" t="s">
+      <c r="G37" s="3"/>
+      <c r="H37" s="3"/>
+      <c r="I37" s="3"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
+      <c r="N37" s="3"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="R37" s="3"/>
+    </row>
+    <row r="38" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>16</v>
+      </c>
+      <c r="B38" s="3">
+        <v>330</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E37" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="G37" s="2"/>
-      <c r="H37" s="2"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="2"/>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
-      <c r="P37" s="2"/>
-      <c r="Q37" s="2" t="s">
+      <c r="D38" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="R37" s="2"/>
-    </row>
-    <row r="38" spans="1:18" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
-        <v>16</v>
-      </c>
-      <c r="B38" s="2">
-        <v>330</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q38" s="2" t="s">
-        <v>136</v>
+      <c r="Q38" s="3" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -2980,22 +2825,22 @@
         <v>2</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="Q39" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
     <row r="40" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3003,22 +2848,22 @@
         <v>2</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q40" s="3" t="s">
         <v>137</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>138</v>
-      </c>
-      <c r="F40" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q40" s="3" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -3026,73 +2871,73 @@
         <v>1</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D41" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>22</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="E41" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" s="2">
-        <v>22</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="G42" s="2"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
-      <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
-      <c r="Q42" s="2" t="s">
+      <c r="D42" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="R42" s="2"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3"/>
+      <c r="O42" s="3"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="R42" s="3"/>
     </row>
     <row r="43" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>3</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>219</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G43" s="3"/>
       <c r="H43" s="3"/>
@@ -3105,7 +2950,7 @@
       <c r="O43" s="3"/>
       <c r="P43" s="3"/>
       <c r="Q43" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="R43" s="3"/>
     </row>
@@ -3114,19 +2959,19 @@
         <v>8</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="G44" s="3"/>
       <c r="H44" s="3"/>
@@ -3139,7 +2984,7 @@
       <c r="O44" s="3"/>
       <c r="P44" s="3"/>
       <c r="Q44" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="R44" s="3"/>
     </row>
@@ -3148,19 +2993,19 @@
         <v>2</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="G45" s="3"/>
       <c r="H45" s="3"/>
@@ -3175,56 +3020,56 @@
       <c r="Q45" s="3"/>
       <c r="R45" s="3"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+    <row r="46" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
         <v>4</v>
       </c>
-      <c r="B46" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="F46" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G46" s="2"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="2"/>
-      <c r="L46" s="2"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="2"/>
-      <c r="O46" s="2"/>
-      <c r="P46" s="2"/>
-      <c r="Q46" s="2"/>
-      <c r="R46" s="2"/>
+      <c r="B46" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G46" s="3"/>
+      <c r="H46" s="3"/>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="3"/>
+      <c r="N46" s="3"/>
+      <c r="O46" s="3"/>
+      <c r="P46" s="3"/>
+      <c r="Q46" s="3"/>
+      <c r="R46" s="3"/>
     </row>
     <row r="47" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>2</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="G47" s="3"/>
       <c r="H47" s="3"/>
@@ -3244,35 +3089,35 @@
         <v>1</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="J48" s="3" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="K48" s="3"/>
       <c r="L48" s="3" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="M48" s="3"/>
       <c r="N48" s="3"/>
@@ -3286,35 +3131,35 @@
         <v>1</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="H49" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="J49" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="J49" s="3" t="s">
-        <v>164</v>
       </c>
       <c r="K49" s="3"/>
       <c r="L49" s="3" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="M49" s="3"/>
       <c r="N49" s="3"/>
@@ -3328,19 +3173,19 @@
         <v>1</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G50" s="3"/>
       <c r="H50" s="3"/>
@@ -3360,19 +3205,19 @@
         <v>1</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G51" s="3"/>
       <c r="H51" s="3"/>
@@ -3387,152 +3232,152 @@
       <c r="Q51" s="3"/>
       <c r="R51" s="3"/>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A52" s="2">
-        <v>1</v>
-      </c>
-      <c r="B52" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E52" s="2" t="s">
+    <row r="52" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>1</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="F52" s="3" t="s">
         <v>178</v>
       </c>
-      <c r="F52" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G52" s="2"/>
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="2"/>
-      <c r="L52" s="2"/>
-      <c r="M52" s="2"/>
-      <c r="N52" s="2"/>
-      <c r="O52" s="2"/>
-      <c r="P52" s="2"/>
-      <c r="Q52" s="2"/>
-      <c r="R52" s="2"/>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A53" s="2">
-        <v>1</v>
-      </c>
-      <c r="B53" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>180</v>
-      </c>
-      <c r="F53" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G53" s="2"/>
-      <c r="H53" s="2"/>
-      <c r="I53" s="2"/>
-      <c r="J53" s="2"/>
-      <c r="K53" s="2"/>
-      <c r="L53" s="2"/>
-      <c r="M53" s="2"/>
-      <c r="N53" s="2"/>
-      <c r="O53" s="2"/>
-      <c r="P53" s="2"/>
-      <c r="Q53" s="2"/>
-      <c r="R53" s="2"/>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A54" s="2">
-        <v>1</v>
-      </c>
-      <c r="B54" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>182</v>
-      </c>
-      <c r="F54" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G54" s="2"/>
-      <c r="H54" s="2"/>
-      <c r="I54" s="2"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="2"/>
-      <c r="L54" s="2"/>
-      <c r="M54" s="2"/>
-      <c r="N54" s="2"/>
-      <c r="O54" s="2"/>
-      <c r="P54" s="2"/>
-      <c r="Q54" s="2"/>
-      <c r="R54" s="2"/>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A55" s="2">
-        <v>1</v>
-      </c>
-      <c r="B55" s="2" t="s">
+      <c r="G52" s="3"/>
+      <c r="H52" s="3"/>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="3"/>
+      <c r="P52" s="3"/>
+      <c r="Q52" s="3"/>
+      <c r="R52" s="3"/>
+    </row>
+    <row r="53" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <v>1</v>
+      </c>
+      <c r="B53" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E55" s="2" t="s">
+      <c r="C53" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E53" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="F55" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G55" s="2"/>
-      <c r="H55" s="2"/>
-      <c r="I55" s="2"/>
-      <c r="J55" s="2"/>
-      <c r="K55" s="2"/>
-      <c r="L55" s="2"/>
-      <c r="M55" s="2"/>
-      <c r="N55" s="2"/>
-      <c r="O55" s="2"/>
-      <c r="P55" s="2"/>
-      <c r="Q55" s="2"/>
-      <c r="R55" s="2"/>
+      <c r="F53" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G53" s="3"/>
+      <c r="H53" s="3"/>
+      <c r="I53" s="3"/>
+      <c r="J53" s="3"/>
+      <c r="K53" s="3"/>
+      <c r="L53" s="3"/>
+      <c r="M53" s="3"/>
+      <c r="N53" s="3"/>
+      <c r="O53" s="3"/>
+      <c r="P53" s="3"/>
+      <c r="Q53" s="3"/>
+      <c r="R53" s="3"/>
+    </row>
+    <row r="54" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <v>1</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G54" s="3"/>
+      <c r="H54" s="3"/>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="3"/>
+      <c r="N54" s="3"/>
+      <c r="O54" s="3"/>
+      <c r="P54" s="3"/>
+      <c r="Q54" s="3"/>
+      <c r="R54" s="3"/>
+    </row>
+    <row r="55" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>1</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="3"/>
+      <c r="O55" s="3"/>
+      <c r="P55" s="3"/>
+      <c r="Q55" s="3"/>
+      <c r="R55" s="3"/>
     </row>
     <row r="56" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>1</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G56" s="3"/>
       <c r="H56" s="3"/>
@@ -3547,56 +3392,56 @@
       <c r="Q56" s="3"/>
       <c r="R56" s="3"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A57" s="2">
-        <v>1</v>
-      </c>
-      <c r="B57" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C57" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
-      <c r="I57" s="2"/>
-      <c r="J57" s="2"/>
-      <c r="K57" s="2"/>
-      <c r="L57" s="2"/>
-      <c r="M57" s="2"/>
-      <c r="N57" s="2"/>
-      <c r="O57" s="2"/>
-      <c r="P57" s="2"/>
-      <c r="Q57" s="2"/>
-      <c r="R57" s="2"/>
+    <row r="57" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <v>1</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G57" s="3"/>
+      <c r="H57" s="3"/>
+      <c r="I57" s="3"/>
+      <c r="J57" s="3"/>
+      <c r="K57" s="3"/>
+      <c r="L57" s="3"/>
+      <c r="M57" s="3"/>
+      <c r="N57" s="3"/>
+      <c r="O57" s="3"/>
+      <c r="P57" s="3"/>
+      <c r="Q57" s="3"/>
+      <c r="R57" s="3"/>
     </row>
     <row r="58" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>1</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G58" s="3"/>
       <c r="H58" s="3"/>
@@ -3616,19 +3461,19 @@
         <v>1</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="F59" s="3" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G59" s="3"/>
       <c r="H59" s="3"/>
@@ -3643,120 +3488,96 @@
       <c r="Q59" s="3"/>
       <c r="R59" s="3"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A60" s="2">
-        <v>1</v>
-      </c>
-      <c r="B60" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="F60" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G60" s="2"/>
-      <c r="H60" s="2"/>
-      <c r="I60" s="2"/>
-      <c r="J60" s="2"/>
-      <c r="K60" s="2"/>
-      <c r="L60" s="2"/>
-      <c r="M60" s="2"/>
-      <c r="N60" s="2"/>
-      <c r="O60" s="2"/>
-      <c r="P60" s="2"/>
-      <c r="Q60" s="2"/>
-      <c r="R60" s="2"/>
-    </row>
-    <row r="61" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>1</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="3"/>
+      <c r="N60" s="3"/>
+      <c r="O60" s="3"/>
+      <c r="P60" s="3"/>
+      <c r="Q60" s="3"/>
+      <c r="R60" s="3"/>
+    </row>
+    <row r="61" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>1</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
-      <c r="J61" s="3"/>
-      <c r="K61" s="3"/>
-      <c r="L61" s="3"/>
-      <c r="M61" s="3"/>
-      <c r="N61" s="3"/>
-      <c r="O61" s="3"/>
-      <c r="P61" s="3"/>
-      <c r="Q61" s="3"/>
-      <c r="R61" s="3"/>
-    </row>
-    <row r="62" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>1</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
-      <c r="J62" s="3"/>
-      <c r="K62" s="3"/>
-      <c r="L62" s="3"/>
-      <c r="M62" s="3"/>
-      <c r="N62" s="3"/>
-      <c r="O62" s="3"/>
-      <c r="P62" s="3"/>
-      <c r="Q62" s="3"/>
-      <c r="R62" s="3"/>
+        <v>178</v>
+      </c>
     </row>
     <row r="63" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>1</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G63" s="3"/>
       <c r="H63" s="3"/>
@@ -3776,19 +3597,19 @@
         <v>1</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G64" s="3"/>
       <c r="H64" s="3"/>
@@ -3808,19 +3629,19 @@
         <v>1</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G65" s="3"/>
       <c r="H65" s="3"/>
@@ -3835,88 +3656,88 @@
       <c r="Q65" s="3"/>
       <c r="R65" s="3"/>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A66" s="2">
-        <v>1</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="C66" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D66" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E66" s="2" t="s">
-        <v>206</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G66" s="2"/>
-      <c r="H66" s="2"/>
-      <c r="I66" s="2"/>
-      <c r="J66" s="2"/>
-      <c r="K66" s="2"/>
-      <c r="L66" s="2"/>
-      <c r="M66" s="2"/>
-      <c r="N66" s="2"/>
-      <c r="O66" s="2"/>
-      <c r="P66" s="2"/>
-      <c r="Q66" s="2"/>
-      <c r="R66" s="2"/>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A67" s="2">
-        <v>1</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>208</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>174</v>
-      </c>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
-      <c r="J67" s="2"/>
-      <c r="K67" s="2"/>
-      <c r="L67" s="2"/>
-      <c r="M67" s="2"/>
-      <c r="N67" s="2"/>
-      <c r="O67" s="2"/>
-      <c r="P67" s="2"/>
-      <c r="Q67" s="2"/>
-      <c r="R67" s="2"/>
+    <row r="66" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="3">
+        <v>1</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E66" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G66" s="3"/>
+      <c r="H66" s="3"/>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+      <c r="L66" s="3"/>
+      <c r="M66" s="3"/>
+      <c r="N66" s="3"/>
+      <c r="O66" s="3"/>
+      <c r="P66" s="3"/>
+      <c r="Q66" s="3"/>
+      <c r="R66" s="3"/>
+    </row>
+    <row r="67" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
+        <v>1</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D67" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E67" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="G67" s="3"/>
+      <c r="H67" s="3"/>
+      <c r="I67" s="3"/>
+      <c r="J67" s="3"/>
+      <c r="K67" s="3"/>
+      <c r="L67" s="3"/>
+      <c r="M67" s="3"/>
+      <c r="N67" s="3"/>
+      <c r="O67" s="3"/>
+      <c r="P67" s="3"/>
+      <c r="Q67" s="3"/>
+      <c r="R67" s="3"/>
     </row>
     <row r="68" spans="1:18" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>1</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="G68" s="3"/>
       <c r="H68" s="3"/>

</xml_diff>